<commit_message>
third iteration - cleaned up and organized
</commit_message>
<xml_diff>
--- a/03_generated_dataset.xlsx
+++ b/03_generated_dataset.xlsx
@@ -1,20 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\grants\2019-08-22 smart cities REU\2025\non-shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2025REU\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715C1C6C-450A-420E-B441-1329261DA142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Travel_Time_Samples_with_Traffi" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -48,7 +62,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -581,26 +595,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -609,6 +607,21 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -930,87 +943,87 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="5" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="5" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="5" t="s">
+      <c r="I1" s="7"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="7"/>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="9" t="s">
+      <c r="L1" s="7"/>
+      <c r="M1" s="8"/>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="10"/>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" s="2">
         <v>15</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <v>15</v>
       </c>
       <c r="D3" s="1">
@@ -1019,7 +1032,7 @@
       <c r="E3" s="2">
         <v>7</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3">
         <v>13</v>
       </c>
       <c r="G3" s="1">
@@ -1028,7 +1041,7 @@
       <c r="H3" s="2">
         <v>12</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3">
         <v>20</v>
       </c>
       <c r="J3" s="1">
@@ -1037,21 +1050,21 @@
       <c r="K3" s="2">
         <v>1</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3">
         <v>2</v>
       </c>
       <c r="M3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="2">
         <v>8</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4">
         <v>12</v>
       </c>
       <c r="D4" s="1">
@@ -1060,7 +1073,7 @@
       <c r="E4" s="2">
         <v>15</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4">
         <v>11</v>
       </c>
       <c r="G4" s="1">
@@ -1069,7 +1082,7 @@
       <c r="H4" s="2">
         <v>8</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4">
         <v>11</v>
       </c>
       <c r="J4" s="1">
@@ -1078,21 +1091,21 @@
       <c r="K4" s="2">
         <v>1</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4">
         <v>2</v>
       </c>
       <c r="M4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="2">
         <v>12</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>13</v>
       </c>
       <c r="D5" s="1">
@@ -1101,7 +1114,7 @@
       <c r="E5" s="2">
         <v>8</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5">
         <v>20</v>
       </c>
       <c r="G5" s="1">
@@ -1110,7 +1123,7 @@
       <c r="H5" s="2">
         <v>7</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5">
         <v>17</v>
       </c>
       <c r="J5" s="1">
@@ -1119,21 +1132,21 @@
       <c r="K5" s="2">
         <v>2</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5">
         <v>2</v>
       </c>
       <c r="M5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="2">
         <v>6</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>17</v>
       </c>
       <c r="D6" s="1">
@@ -1142,7 +1155,7 @@
       <c r="E6" s="2">
         <v>13</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6">
         <v>10</v>
       </c>
       <c r="G6" s="1">
@@ -1151,7 +1164,7 @@
       <c r="H6" s="2">
         <v>14</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6">
         <v>18</v>
       </c>
       <c r="J6" s="1">
@@ -1160,21 +1173,21 @@
       <c r="K6" s="2">
         <v>1</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6">
         <v>2</v>
       </c>
       <c r="M6" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="2">
         <v>8</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7">
         <v>15</v>
       </c>
       <c r="D7" s="1">
@@ -1183,7 +1196,7 @@
       <c r="E7" s="2">
         <v>9</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7">
         <v>12</v>
       </c>
       <c r="G7" s="1">
@@ -1192,7 +1205,7 @@
       <c r="H7" s="2">
         <v>12</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7">
         <v>10</v>
       </c>
       <c r="J7" s="1">
@@ -1201,21 +1214,21 @@
       <c r="K7" s="2">
         <v>1</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7">
         <v>1</v>
       </c>
       <c r="M7" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="2">
         <v>14</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8">
         <v>16</v>
       </c>
       <c r="D8" s="1">
@@ -1224,7 +1237,7 @@
       <c r="E8" s="2">
         <v>8</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8">
         <v>13</v>
       </c>
       <c r="G8" s="1">
@@ -1233,7 +1246,7 @@
       <c r="H8" s="2">
         <v>7</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8">
         <v>19</v>
       </c>
       <c r="J8" s="1">
@@ -1242,21 +1255,21 @@
       <c r="K8" s="2">
         <v>3</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8">
         <v>1</v>
       </c>
       <c r="M8" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="2">
         <v>15</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9">
         <v>11</v>
       </c>
       <c r="D9" s="1">
@@ -1265,7 +1278,7 @@
       <c r="E9" s="2">
         <v>14</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9">
         <v>12</v>
       </c>
       <c r="G9" s="1">
@@ -1274,7 +1287,7 @@
       <c r="H9" s="2">
         <v>14</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9">
         <v>13</v>
       </c>
       <c r="J9" s="1">
@@ -1283,21 +1296,21 @@
       <c r="K9" s="2">
         <v>2</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9">
         <v>1</v>
       </c>
       <c r="M9" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="2">
         <v>6</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10">
         <v>19</v>
       </c>
       <c r="D10" s="1">
@@ -1306,7 +1319,7 @@
       <c r="E10" s="2">
         <v>14</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10">
         <v>12</v>
       </c>
       <c r="G10" s="1">
@@ -1315,7 +1328,7 @@
       <c r="H10" s="2">
         <v>11</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10">
         <v>18</v>
       </c>
       <c r="J10" s="1">
@@ -1324,21 +1337,21 @@
       <c r="K10" s="2">
         <v>2</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10">
         <v>1</v>
       </c>
       <c r="M10" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>8</v>
       </c>
       <c r="B11" s="2">
         <v>7</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11">
         <v>20</v>
       </c>
       <c r="D11" s="1">
@@ -1347,7 +1360,7 @@
       <c r="E11" s="2">
         <v>7</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11">
         <v>11</v>
       </c>
       <c r="G11" s="1">
@@ -1356,7 +1369,7 @@
       <c r="H11" s="2">
         <v>12</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11">
         <v>19</v>
       </c>
       <c r="J11" s="1">
@@ -1365,21 +1378,21 @@
       <c r="K11" s="2">
         <v>3</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11">
         <v>1</v>
       </c>
       <c r="M11" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12">
         <v>19</v>
       </c>
       <c r="D12" s="1">
@@ -1388,7 +1401,7 @@
       <c r="E12" s="2">
         <v>14</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12">
         <v>12</v>
       </c>
       <c r="G12" s="1">
@@ -1397,7 +1410,7 @@
       <c r="H12" s="2">
         <v>13</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12">
         <v>18</v>
       </c>
       <c r="J12" s="1">
@@ -1406,21 +1419,21 @@
       <c r="K12" s="2">
         <v>2</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12">
         <v>2</v>
       </c>
       <c r="M12" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13" s="2">
         <v>13</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13">
         <v>15</v>
       </c>
       <c r="D13" s="1">
@@ -1429,7 +1442,7 @@
       <c r="E13" s="2">
         <v>10</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13">
         <v>19</v>
       </c>
       <c r="G13" s="1">
@@ -1438,7 +1451,7 @@
       <c r="H13" s="2">
         <v>7</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13">
         <v>16</v>
       </c>
       <c r="J13" s="1">
@@ -1447,21 +1460,21 @@
       <c r="K13" s="2">
         <v>2</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13">
         <v>2</v>
       </c>
       <c r="M13" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" s="2">
         <v>15</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14">
         <v>10</v>
       </c>
       <c r="D14" s="1">
@@ -1470,7 +1483,7 @@
       <c r="E14" s="2">
         <v>6</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14">
         <v>19</v>
       </c>
       <c r="G14" s="1">
@@ -1479,7 +1492,7 @@
       <c r="H14" s="2">
         <v>14</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14">
         <v>18</v>
       </c>
       <c r="J14" s="1">
@@ -1488,21 +1501,21 @@
       <c r="K14" s="2">
         <v>3</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14">
         <v>3</v>
       </c>
       <c r="M14" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>12</v>
       </c>
       <c r="B15" s="2">
         <v>6</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15">
         <v>19</v>
       </c>
       <c r="D15" s="1">
@@ -1511,7 +1524,7 @@
       <c r="E15" s="2">
         <v>12</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15">
         <v>15</v>
       </c>
       <c r="G15" s="1">
@@ -1520,7 +1533,7 @@
       <c r="H15" s="2">
         <v>10</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15">
         <v>10</v>
       </c>
       <c r="J15" s="1">
@@ -1529,21 +1542,21 @@
       <c r="K15" s="2">
         <v>1</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15">
         <v>3</v>
       </c>
       <c r="M15" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>13</v>
       </c>
       <c r="B16" s="2">
         <v>7</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16">
         <v>12</v>
       </c>
       <c r="D16" s="1">
@@ -1552,7 +1565,7 @@
       <c r="E16" s="2">
         <v>11</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16">
         <v>11</v>
       </c>
       <c r="G16" s="1">
@@ -1561,7 +1574,7 @@
       <c r="H16" s="2">
         <v>11</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16">
         <v>10</v>
       </c>
       <c r="J16" s="1">
@@ -1570,21 +1583,21 @@
       <c r="K16" s="2">
         <v>2</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L16">
         <v>2</v>
       </c>
       <c r="M16" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>14</v>
       </c>
       <c r="B17" s="2">
         <v>6</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17">
         <v>10</v>
       </c>
       <c r="D17" s="1">
@@ -1593,7 +1606,7 @@
       <c r="E17" s="2">
         <v>14</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17">
         <v>11</v>
       </c>
       <c r="G17" s="1">
@@ -1602,7 +1615,7 @@
       <c r="H17" s="2">
         <v>14</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17">
         <v>20</v>
       </c>
       <c r="J17" s="1">
@@ -1611,21 +1624,21 @@
       <c r="K17" s="2">
         <v>1</v>
       </c>
-      <c r="L17" s="3">
+      <c r="L17">
         <v>2</v>
       </c>
       <c r="M17" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>15</v>
       </c>
       <c r="B18" s="2">
         <v>8</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18">
         <v>13</v>
       </c>
       <c r="D18" s="1">
@@ -1634,7 +1647,7 @@
       <c r="E18" s="2">
         <v>12</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18">
         <v>11</v>
       </c>
       <c r="G18" s="1">
@@ -1643,7 +1656,7 @@
       <c r="H18" s="2">
         <v>15</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18">
         <v>12</v>
       </c>
       <c r="J18" s="1">
@@ -1652,21 +1665,21 @@
       <c r="K18" s="2">
         <v>3</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18">
         <v>2</v>
       </c>
       <c r="M18" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>16</v>
       </c>
       <c r="B19" s="2">
         <v>7</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19">
         <v>17</v>
       </c>
       <c r="D19" s="1">
@@ -1675,7 +1688,7 @@
       <c r="E19" s="2">
         <v>12</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19">
         <v>16</v>
       </c>
       <c r="G19" s="1">
@@ -1684,7 +1697,7 @@
       <c r="H19" s="2">
         <v>7</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19">
         <v>17</v>
       </c>
       <c r="J19" s="1">
@@ -1693,21 +1706,21 @@
       <c r="K19" s="2">
         <v>1</v>
       </c>
-      <c r="L19" s="3">
+      <c r="L19">
         <v>2</v>
       </c>
       <c r="M19" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>17</v>
       </c>
       <c r="B20" s="2">
         <v>14</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20">
         <v>20</v>
       </c>
       <c r="D20" s="1">
@@ -1716,7 +1729,7 @@
       <c r="E20" s="2">
         <v>7</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20">
         <v>10</v>
       </c>
       <c r="G20" s="1">
@@ -1725,7 +1738,7 @@
       <c r="H20" s="2">
         <v>7</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20">
         <v>17</v>
       </c>
       <c r="J20" s="1">
@@ -1734,21 +1747,21 @@
       <c r="K20" s="2">
         <v>1</v>
       </c>
-      <c r="L20" s="3">
+      <c r="L20">
         <v>1</v>
       </c>
       <c r="M20" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>18</v>
       </c>
       <c r="B21" s="2">
         <v>9</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21">
         <v>17</v>
       </c>
       <c r="D21" s="1">
@@ -1757,7 +1770,7 @@
       <c r="E21" s="2">
         <v>13</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21">
         <v>10</v>
       </c>
       <c r="G21" s="1">
@@ -1766,7 +1779,7 @@
       <c r="H21" s="2">
         <v>13</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21">
         <v>10</v>
       </c>
       <c r="J21" s="1">
@@ -1775,21 +1788,21 @@
       <c r="K21" s="2">
         <v>2</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21">
         <v>3</v>
       </c>
       <c r="M21" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>19</v>
       </c>
       <c r="B22" s="2">
         <v>15</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22">
         <v>10</v>
       </c>
       <c r="D22" s="1">
@@ -1798,7 +1811,7 @@
       <c r="E22" s="2">
         <v>12</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22">
         <v>14</v>
       </c>
       <c r="G22" s="1">
@@ -1807,7 +1820,7 @@
       <c r="H22" s="2">
         <v>9</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22">
         <v>12</v>
       </c>
       <c r="J22" s="1">
@@ -1816,21 +1829,21 @@
       <c r="K22" s="2">
         <v>1</v>
       </c>
-      <c r="L22" s="3">
+      <c r="L22">
         <v>2</v>
       </c>
       <c r="M22" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>20</v>
       </c>
       <c r="B23" s="2">
         <v>7</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23">
         <v>16</v>
       </c>
       <c r="D23" s="1">
@@ -1839,7 +1852,7 @@
       <c r="E23" s="2">
         <v>10</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23">
         <v>14</v>
       </c>
       <c r="G23" s="1">
@@ -1848,7 +1861,7 @@
       <c r="H23" s="2">
         <v>8</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23">
         <v>20</v>
       </c>
       <c r="J23" s="1">
@@ -1857,21 +1870,21 @@
       <c r="K23" s="2">
         <v>2</v>
       </c>
-      <c r="L23" s="3">
+      <c r="L23">
         <v>1</v>
       </c>
       <c r="M23" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>21</v>
       </c>
       <c r="B24" s="2">
         <v>15</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24">
         <v>16</v>
       </c>
       <c r="D24" s="1">
@@ -1880,7 +1893,7 @@
       <c r="E24" s="2">
         <v>11</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24">
         <v>14</v>
       </c>
       <c r="G24" s="1">
@@ -1889,7 +1902,7 @@
       <c r="H24" s="2">
         <v>12</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24">
         <v>11</v>
       </c>
       <c r="J24" s="1">
@@ -1898,21 +1911,21 @@
       <c r="K24" s="2">
         <v>2</v>
       </c>
-      <c r="L24" s="3">
+      <c r="L24">
         <v>2</v>
       </c>
       <c r="M24" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>22</v>
       </c>
       <c r="B25" s="2">
         <v>6</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25">
         <v>20</v>
       </c>
       <c r="D25" s="1">
@@ -1921,7 +1934,7 @@
       <c r="E25" s="2">
         <v>13</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25">
         <v>13</v>
       </c>
       <c r="G25" s="1">
@@ -1930,7 +1943,7 @@
       <c r="H25" s="2">
         <v>7</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25">
         <v>17</v>
       </c>
       <c r="J25" s="1">
@@ -1939,21 +1952,21 @@
       <c r="K25" s="2">
         <v>2</v>
       </c>
-      <c r="L25" s="3">
+      <c r="L25">
         <v>2</v>
       </c>
       <c r="M25" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>23</v>
       </c>
       <c r="B26" s="2">
         <v>9</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26">
         <v>10</v>
       </c>
       <c r="D26" s="1">
@@ -1962,7 +1975,7 @@
       <c r="E26" s="2">
         <v>15</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26">
         <v>20</v>
       </c>
       <c r="G26" s="1">
@@ -1971,7 +1984,7 @@
       <c r="H26" s="2">
         <v>13</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26">
         <v>12</v>
       </c>
       <c r="J26" s="1">
@@ -1980,21 +1993,21 @@
       <c r="K26" s="2">
         <v>3</v>
       </c>
-      <c r="L26" s="3">
+      <c r="L26">
         <v>2</v>
       </c>
       <c r="M26" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>24</v>
       </c>
       <c r="B27" s="2">
         <v>6</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27">
         <v>14</v>
       </c>
       <c r="D27" s="1">
@@ -2003,7 +2016,7 @@
       <c r="E27" s="2">
         <v>12</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27">
         <v>15</v>
       </c>
       <c r="G27" s="1">
@@ -2012,7 +2025,7 @@
       <c r="H27" s="2">
         <v>7</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27">
         <v>18</v>
       </c>
       <c r="J27" s="1">
@@ -2021,21 +2034,21 @@
       <c r="K27" s="2">
         <v>2</v>
       </c>
-      <c r="L27" s="3">
+      <c r="L27">
         <v>3</v>
       </c>
       <c r="M27" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>25</v>
       </c>
       <c r="B28" s="2">
         <v>13</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28">
         <v>19</v>
       </c>
       <c r="D28" s="1">
@@ -2044,7 +2057,7 @@
       <c r="E28" s="2">
         <v>9</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28">
         <v>19</v>
       </c>
       <c r="G28" s="1">
@@ -2053,7 +2066,7 @@
       <c r="H28" s="2">
         <v>13</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28">
         <v>14</v>
       </c>
       <c r="J28" s="1">
@@ -2062,21 +2075,21 @@
       <c r="K28" s="2">
         <v>2</v>
       </c>
-      <c r="L28" s="3">
+      <c r="L28">
         <v>2</v>
       </c>
       <c r="M28" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>26</v>
       </c>
       <c r="B29" s="2">
         <v>7</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29">
         <v>18</v>
       </c>
       <c r="D29" s="1">
@@ -2085,7 +2098,7 @@
       <c r="E29" s="2">
         <v>15</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29">
         <v>19</v>
       </c>
       <c r="G29" s="1">
@@ -2094,7 +2107,7 @@
       <c r="H29" s="2">
         <v>9</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29">
         <v>16</v>
       </c>
       <c r="J29" s="1">
@@ -2103,21 +2116,21 @@
       <c r="K29" s="2">
         <v>2</v>
       </c>
-      <c r="L29" s="3">
+      <c r="L29">
         <v>1</v>
       </c>
       <c r="M29" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>27</v>
       </c>
       <c r="B30" s="2">
         <v>6</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30">
         <v>20</v>
       </c>
       <c r="D30" s="1">
@@ -2126,7 +2139,7 @@
       <c r="E30" s="2">
         <v>8</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30">
         <v>14</v>
       </c>
       <c r="G30" s="1">
@@ -2135,7 +2148,7 @@
       <c r="H30" s="2">
         <v>14</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30">
         <v>11</v>
       </c>
       <c r="J30" s="1">
@@ -2144,21 +2157,21 @@
       <c r="K30" s="2">
         <v>2</v>
       </c>
-      <c r="L30" s="3">
+      <c r="L30">
         <v>1</v>
       </c>
       <c r="M30" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>28</v>
       </c>
       <c r="B31" s="2">
         <v>6</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31">
         <v>12</v>
       </c>
       <c r="D31" s="1">
@@ -2167,7 +2180,7 @@
       <c r="E31" s="2">
         <v>8</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31">
         <v>17</v>
       </c>
       <c r="G31" s="1">
@@ -2176,7 +2189,7 @@
       <c r="H31" s="2">
         <v>13</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31">
         <v>18</v>
       </c>
       <c r="J31" s="1">
@@ -2185,21 +2198,21 @@
       <c r="K31" s="2">
         <v>2</v>
       </c>
-      <c r="L31" s="3">
+      <c r="L31">
         <v>2</v>
       </c>
       <c r="M31" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>29</v>
       </c>
       <c r="B32" s="2">
         <v>8</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32">
         <v>20</v>
       </c>
       <c r="D32" s="1">
@@ -2208,7 +2221,7 @@
       <c r="E32" s="2">
         <v>8</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32">
         <v>16</v>
       </c>
       <c r="G32" s="1">
@@ -2217,7 +2230,7 @@
       <c r="H32" s="2">
         <v>10</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32">
         <v>12</v>
       </c>
       <c r="J32" s="1">
@@ -2226,21 +2239,21 @@
       <c r="K32" s="2">
         <v>3</v>
       </c>
-      <c r="L32" s="3">
+      <c r="L32">
         <v>1</v>
       </c>
       <c r="M32" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>30</v>
       </c>
       <c r="B33" s="2">
         <v>12</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33">
         <v>20</v>
       </c>
       <c r="D33" s="1">
@@ -2249,7 +2262,7 @@
       <c r="E33" s="2">
         <v>7</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33">
         <v>14</v>
       </c>
       <c r="G33" s="1">
@@ -2258,7 +2271,7 @@
       <c r="H33" s="2">
         <v>10</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I33">
         <v>13</v>
       </c>
       <c r="J33" s="1">
@@ -2267,21 +2280,21 @@
       <c r="K33" s="2">
         <v>1</v>
       </c>
-      <c r="L33" s="3">
+      <c r="L33">
         <v>2</v>
       </c>
       <c r="M33" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>31</v>
       </c>
       <c r="B34" s="2">
         <v>13</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34">
         <v>16</v>
       </c>
       <c r="D34" s="1">
@@ -2290,7 +2303,7 @@
       <c r="E34" s="2">
         <v>8</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34">
         <v>10</v>
       </c>
       <c r="G34" s="1">
@@ -2299,7 +2312,7 @@
       <c r="H34" s="2">
         <v>10</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34">
         <v>19</v>
       </c>
       <c r="J34" s="1">
@@ -2308,21 +2321,21 @@
       <c r="K34" s="2">
         <v>1</v>
       </c>
-      <c r="L34" s="3">
+      <c r="L34">
         <v>1</v>
       </c>
       <c r="M34" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>32</v>
       </c>
       <c r="B35" s="2">
         <v>12</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35">
         <v>17</v>
       </c>
       <c r="D35" s="1">
@@ -2331,7 +2344,7 @@
       <c r="E35" s="2">
         <v>13</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35">
         <v>20</v>
       </c>
       <c r="G35" s="1">
@@ -2340,7 +2353,7 @@
       <c r="H35" s="2">
         <v>8</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35">
         <v>17</v>
       </c>
       <c r="J35" s="1">
@@ -2349,21 +2362,21 @@
       <c r="K35" s="2">
         <v>2</v>
       </c>
-      <c r="L35" s="3">
+      <c r="L35">
         <v>1</v>
       </c>
       <c r="M35" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>33</v>
       </c>
       <c r="B36" s="2">
         <v>7</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36">
         <v>11</v>
       </c>
       <c r="D36" s="1">
@@ -2372,7 +2385,7 @@
       <c r="E36" s="2">
         <v>6</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36">
         <v>15</v>
       </c>
       <c r="G36" s="1">
@@ -2381,7 +2394,7 @@
       <c r="H36" s="2">
         <v>6</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I36">
         <v>17</v>
       </c>
       <c r="J36" s="1">
@@ -2390,21 +2403,21 @@
       <c r="K36" s="2">
         <v>3</v>
       </c>
-      <c r="L36" s="3">
+      <c r="L36">
         <v>2</v>
       </c>
       <c r="M36" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>34</v>
       </c>
       <c r="B37" s="2">
         <v>8</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37">
         <v>17</v>
       </c>
       <c r="D37" s="1">
@@ -2413,7 +2426,7 @@
       <c r="E37" s="2">
         <v>11</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37">
         <v>15</v>
       </c>
       <c r="G37" s="1">
@@ -2422,7 +2435,7 @@
       <c r="H37" s="2">
         <v>8</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I37">
         <v>18</v>
       </c>
       <c r="J37" s="1">
@@ -2431,21 +2444,21 @@
       <c r="K37" s="2">
         <v>1</v>
       </c>
-      <c r="L37" s="3">
+      <c r="L37">
         <v>2</v>
       </c>
       <c r="M37" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>35</v>
       </c>
       <c r="B38" s="2">
         <v>8</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38">
         <v>11</v>
       </c>
       <c r="D38" s="1">
@@ -2454,7 +2467,7 @@
       <c r="E38" s="2">
         <v>14</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38">
         <v>18</v>
       </c>
       <c r="G38" s="1">
@@ -2463,7 +2476,7 @@
       <c r="H38" s="2">
         <v>14</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38">
         <v>13</v>
       </c>
       <c r="J38" s="1">
@@ -2472,21 +2485,21 @@
       <c r="K38" s="2">
         <v>2</v>
       </c>
-      <c r="L38" s="3">
+      <c r="L38">
         <v>2</v>
       </c>
       <c r="M38" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>36</v>
       </c>
       <c r="B39" s="2">
         <v>7</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39">
         <v>13</v>
       </c>
       <c r="D39" s="1">
@@ -2495,7 +2508,7 @@
       <c r="E39" s="2">
         <v>15</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39">
         <v>10</v>
       </c>
       <c r="G39" s="1">
@@ -2504,7 +2517,7 @@
       <c r="H39" s="2">
         <v>15</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I39">
         <v>17</v>
       </c>
       <c r="J39" s="1">
@@ -2513,21 +2526,21 @@
       <c r="K39" s="2">
         <v>3</v>
       </c>
-      <c r="L39" s="3">
+      <c r="L39">
         <v>1</v>
       </c>
       <c r="M39" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>37</v>
       </c>
       <c r="B40" s="2">
         <v>8</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40">
         <v>19</v>
       </c>
       <c r="D40" s="1">
@@ -2536,7 +2549,7 @@
       <c r="E40" s="2">
         <v>6</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40">
         <v>19</v>
       </c>
       <c r="G40" s="1">
@@ -2545,7 +2558,7 @@
       <c r="H40" s="2">
         <v>7</v>
       </c>
-      <c r="I40" s="3">
+      <c r="I40">
         <v>13</v>
       </c>
       <c r="J40" s="1">
@@ -2554,21 +2567,21 @@
       <c r="K40" s="2">
         <v>3</v>
       </c>
-      <c r="L40" s="3">
+      <c r="L40">
         <v>3</v>
       </c>
       <c r="M40" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>38</v>
       </c>
       <c r="B41" s="2">
         <v>6</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41">
         <v>20</v>
       </c>
       <c r="D41" s="1">
@@ -2577,7 +2590,7 @@
       <c r="E41" s="2">
         <v>15</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41">
         <v>11</v>
       </c>
       <c r="G41" s="1">
@@ -2586,7 +2599,7 @@
       <c r="H41" s="2">
         <v>8</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I41">
         <v>13</v>
       </c>
       <c r="J41" s="1">
@@ -2595,21 +2608,21 @@
       <c r="K41" s="2">
         <v>2</v>
       </c>
-      <c r="L41" s="3">
+      <c r="L41">
         <v>2</v>
       </c>
       <c r="M41" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>39</v>
       </c>
       <c r="B42" s="2">
         <v>8</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42">
         <v>18</v>
       </c>
       <c r="D42" s="1">
@@ -2618,7 +2631,7 @@
       <c r="E42" s="2">
         <v>13</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42">
         <v>11</v>
       </c>
       <c r="G42" s="1">
@@ -2627,7 +2640,7 @@
       <c r="H42" s="2">
         <v>7</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I42">
         <v>16</v>
       </c>
       <c r="J42" s="1">
@@ -2636,21 +2649,21 @@
       <c r="K42" s="2">
         <v>1</v>
       </c>
-      <c r="L42" s="3">
+      <c r="L42">
         <v>2</v>
       </c>
       <c r="M42" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>40</v>
       </c>
       <c r="B43" s="2">
         <v>9</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43">
         <v>18</v>
       </c>
       <c r="D43" s="1">
@@ -2659,7 +2672,7 @@
       <c r="E43" s="2">
         <v>7</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43">
         <v>18</v>
       </c>
       <c r="G43" s="1">
@@ -2668,7 +2681,7 @@
       <c r="H43" s="2">
         <v>9</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I43">
         <v>13</v>
       </c>
       <c r="J43" s="1">
@@ -2677,21 +2690,21 @@
       <c r="K43" s="2">
         <v>2</v>
       </c>
-      <c r="L43" s="3">
+      <c r="L43">
         <v>2</v>
       </c>
       <c r="M43" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>41</v>
       </c>
       <c r="B44" s="2">
         <v>9</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44">
         <v>14</v>
       </c>
       <c r="D44" s="1">
@@ -2700,7 +2713,7 @@
       <c r="E44" s="2">
         <v>7</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44">
         <v>15</v>
       </c>
       <c r="G44" s="1">
@@ -2709,7 +2722,7 @@
       <c r="H44" s="2">
         <v>15</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I44">
         <v>15</v>
       </c>
       <c r="J44" s="1">
@@ -2718,21 +2731,21 @@
       <c r="K44" s="2">
         <v>3</v>
       </c>
-      <c r="L44" s="3">
+      <c r="L44">
         <v>2</v>
       </c>
       <c r="M44" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>42</v>
       </c>
       <c r="B45" s="2">
         <v>8</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45">
         <v>15</v>
       </c>
       <c r="D45" s="1">
@@ -2741,7 +2754,7 @@
       <c r="E45" s="2">
         <v>8</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45">
         <v>19</v>
       </c>
       <c r="G45" s="1">
@@ -2750,7 +2763,7 @@
       <c r="H45" s="2">
         <v>8</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I45">
         <v>19</v>
       </c>
       <c r="J45" s="1">
@@ -2759,21 +2772,21 @@
       <c r="K45" s="2">
         <v>2</v>
       </c>
-      <c r="L45" s="3">
+      <c r="L45">
         <v>2</v>
       </c>
       <c r="M45" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>43</v>
       </c>
       <c r="B46" s="2">
         <v>14</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46">
         <v>13</v>
       </c>
       <c r="D46" s="1">
@@ -2782,7 +2795,7 @@
       <c r="E46" s="2">
         <v>6</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F46">
         <v>19</v>
       </c>
       <c r="G46" s="1">
@@ -2791,7 +2804,7 @@
       <c r="H46" s="2">
         <v>15</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I46">
         <v>20</v>
       </c>
       <c r="J46" s="1">
@@ -2800,21 +2813,21 @@
       <c r="K46" s="2">
         <v>2</v>
       </c>
-      <c r="L46" s="3">
+      <c r="L46">
         <v>2</v>
       </c>
       <c r="M46" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>44</v>
       </c>
       <c r="B47" s="2">
         <v>8</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47">
         <v>17</v>
       </c>
       <c r="D47" s="1">
@@ -2823,7 +2836,7 @@
       <c r="E47" s="2">
         <v>6</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F47">
         <v>13</v>
       </c>
       <c r="G47" s="1">
@@ -2832,7 +2845,7 @@
       <c r="H47" s="2">
         <v>9</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I47">
         <v>20</v>
       </c>
       <c r="J47" s="1">
@@ -2841,21 +2854,21 @@
       <c r="K47" s="2">
         <v>1</v>
       </c>
-      <c r="L47" s="3">
+      <c r="L47">
         <v>3</v>
       </c>
       <c r="M47" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>45</v>
       </c>
       <c r="B48" s="2">
         <v>7</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48">
         <v>13</v>
       </c>
       <c r="D48" s="1">
@@ -2864,7 +2877,7 @@
       <c r="E48" s="2">
         <v>11</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F48">
         <v>14</v>
       </c>
       <c r="G48" s="1">
@@ -2873,7 +2886,7 @@
       <c r="H48" s="2">
         <v>14</v>
       </c>
-      <c r="I48" s="3">
+      <c r="I48">
         <v>15</v>
       </c>
       <c r="J48" s="1">
@@ -2882,21 +2895,21 @@
       <c r="K48" s="2">
         <v>2</v>
       </c>
-      <c r="L48" s="3">
+      <c r="L48">
         <v>2</v>
       </c>
       <c r="M48" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>46</v>
       </c>
       <c r="B49" s="2">
         <v>6</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49">
         <v>13</v>
       </c>
       <c r="D49" s="1">
@@ -2905,7 +2918,7 @@
       <c r="E49" s="2">
         <v>9</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F49">
         <v>17</v>
       </c>
       <c r="G49" s="1">
@@ -2914,7 +2927,7 @@
       <c r="H49" s="2">
         <v>15</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I49">
         <v>15</v>
       </c>
       <c r="J49" s="1">
@@ -2923,21 +2936,21 @@
       <c r="K49" s="2">
         <v>3</v>
       </c>
-      <c r="L49" s="3">
+      <c r="L49">
         <v>1</v>
       </c>
       <c r="M49" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>47</v>
       </c>
       <c r="B50" s="2">
         <v>9</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50">
         <v>14</v>
       </c>
       <c r="D50" s="1">
@@ -2946,7 +2959,7 @@
       <c r="E50" s="2">
         <v>10</v>
       </c>
-      <c r="F50" s="3">
+      <c r="F50">
         <v>10</v>
       </c>
       <c r="G50" s="1">
@@ -2955,7 +2968,7 @@
       <c r="H50" s="2">
         <v>11</v>
       </c>
-      <c r="I50" s="3">
+      <c r="I50">
         <v>19</v>
       </c>
       <c r="J50" s="1">
@@ -2964,21 +2977,21 @@
       <c r="K50" s="2">
         <v>1</v>
       </c>
-      <c r="L50" s="3">
+      <c r="L50">
         <v>2</v>
       </c>
       <c r="M50" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>48</v>
       </c>
       <c r="B51" s="2">
         <v>7</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51">
         <v>10</v>
       </c>
       <c r="D51" s="1">
@@ -2987,7 +3000,7 @@
       <c r="E51" s="2">
         <v>12</v>
       </c>
-      <c r="F51" s="3">
+      <c r="F51">
         <v>20</v>
       </c>
       <c r="G51" s="1">
@@ -2996,7 +3009,7 @@
       <c r="H51" s="2">
         <v>7</v>
       </c>
-      <c r="I51" s="3">
+      <c r="I51">
         <v>16</v>
       </c>
       <c r="J51" s="1">
@@ -3005,21 +3018,21 @@
       <c r="K51" s="2">
         <v>2</v>
       </c>
-      <c r="L51" s="3">
+      <c r="L51">
         <v>1</v>
       </c>
       <c r="M51" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>49</v>
       </c>
       <c r="B52" s="2">
         <v>11</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52">
         <v>14</v>
       </c>
       <c r="D52" s="1">
@@ -3028,7 +3041,7 @@
       <c r="E52" s="2">
         <v>11</v>
       </c>
-      <c r="F52" s="3">
+      <c r="F52">
         <v>15</v>
       </c>
       <c r="G52" s="1">
@@ -3037,7 +3050,7 @@
       <c r="H52" s="2">
         <v>6</v>
       </c>
-      <c r="I52" s="3">
+      <c r="I52">
         <v>17</v>
       </c>
       <c r="J52" s="1">
@@ -3046,21 +3059,21 @@
       <c r="K52" s="2">
         <v>3</v>
       </c>
-      <c r="L52" s="3">
+      <c r="L52">
         <v>3</v>
       </c>
       <c r="M52" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>50</v>
       </c>
       <c r="B53" s="2">
         <v>7</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53">
         <v>17</v>
       </c>
       <c r="D53" s="1">
@@ -3069,7 +3082,7 @@
       <c r="E53" s="2">
         <v>9</v>
       </c>
-      <c r="F53" s="3">
+      <c r="F53">
         <v>20</v>
       </c>
       <c r="G53" s="1">
@@ -3078,7 +3091,7 @@
       <c r="H53" s="2">
         <v>12</v>
       </c>
-      <c r="I53" s="3">
+      <c r="I53">
         <v>11</v>
       </c>
       <c r="J53" s="1">
@@ -3087,21 +3100,21 @@
       <c r="K53" s="2">
         <v>2</v>
       </c>
-      <c r="L53" s="3">
+      <c r="L53">
         <v>2</v>
       </c>
       <c r="M53" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>51</v>
       </c>
       <c r="B54" s="2">
         <v>14</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54">
         <v>19</v>
       </c>
       <c r="D54" s="1">
@@ -3110,7 +3123,7 @@
       <c r="E54" s="2">
         <v>8</v>
       </c>
-      <c r="F54" s="3">
+      <c r="F54">
         <v>13</v>
       </c>
       <c r="G54" s="1">
@@ -3119,7 +3132,7 @@
       <c r="H54" s="2">
         <v>6</v>
       </c>
-      <c r="I54" s="3">
+      <c r="I54">
         <v>19</v>
       </c>
       <c r="J54" s="1">
@@ -3128,21 +3141,21 @@
       <c r="K54" s="2">
         <v>1</v>
       </c>
-      <c r="L54" s="3">
+      <c r="L54">
         <v>2</v>
       </c>
       <c r="M54" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>52</v>
       </c>
       <c r="B55" s="2">
         <v>9</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55">
         <v>13</v>
       </c>
       <c r="D55" s="1">
@@ -3151,7 +3164,7 @@
       <c r="E55" s="2">
         <v>11</v>
       </c>
-      <c r="F55" s="3">
+      <c r="F55">
         <v>20</v>
       </c>
       <c r="G55" s="1">
@@ -3160,7 +3173,7 @@
       <c r="H55" s="2">
         <v>8</v>
       </c>
-      <c r="I55" s="3">
+      <c r="I55">
         <v>17</v>
       </c>
       <c r="J55" s="1">
@@ -3169,21 +3182,21 @@
       <c r="K55" s="2">
         <v>2</v>
       </c>
-      <c r="L55" s="3">
+      <c r="L55">
         <v>3</v>
       </c>
       <c r="M55" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>53</v>
       </c>
       <c r="B56" s="2">
         <v>10</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56">
         <v>15</v>
       </c>
       <c r="D56" s="1">
@@ -3192,7 +3205,7 @@
       <c r="E56" s="2">
         <v>14</v>
       </c>
-      <c r="F56" s="3">
+      <c r="F56">
         <v>17</v>
       </c>
       <c r="G56" s="1">
@@ -3201,7 +3214,7 @@
       <c r="H56" s="2">
         <v>14</v>
       </c>
-      <c r="I56" s="3">
+      <c r="I56">
         <v>20</v>
       </c>
       <c r="J56" s="1">
@@ -3210,21 +3223,21 @@
       <c r="K56" s="2">
         <v>2</v>
       </c>
-      <c r="L56" s="3">
+      <c r="L56">
         <v>1</v>
       </c>
       <c r="M56" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>54</v>
       </c>
       <c r="B57" s="2">
         <v>10</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C57">
         <v>17</v>
       </c>
       <c r="D57" s="1">
@@ -3233,7 +3246,7 @@
       <c r="E57" s="2">
         <v>12</v>
       </c>
-      <c r="F57" s="3">
+      <c r="F57">
         <v>10</v>
       </c>
       <c r="G57" s="1">
@@ -3242,7 +3255,7 @@
       <c r="H57" s="2">
         <v>13</v>
       </c>
-      <c r="I57" s="3">
+      <c r="I57">
         <v>14</v>
       </c>
       <c r="J57" s="1">
@@ -3251,21 +3264,21 @@
       <c r="K57" s="2">
         <v>2</v>
       </c>
-      <c r="L57" s="3">
+      <c r="L57">
         <v>2</v>
       </c>
       <c r="M57" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>55</v>
       </c>
       <c r="B58" s="2">
         <v>11</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C58">
         <v>14</v>
       </c>
       <c r="D58" s="1">
@@ -3274,7 +3287,7 @@
       <c r="E58" s="2">
         <v>8</v>
       </c>
-      <c r="F58" s="3">
+      <c r="F58">
         <v>13</v>
       </c>
       <c r="G58" s="1">
@@ -3283,7 +3296,7 @@
       <c r="H58" s="2">
         <v>9</v>
       </c>
-      <c r="I58" s="3">
+      <c r="I58">
         <v>12</v>
       </c>
       <c r="J58" s="1">
@@ -3292,21 +3305,21 @@
       <c r="K58" s="2">
         <v>1</v>
       </c>
-      <c r="L58" s="3">
+      <c r="L58">
         <v>3</v>
       </c>
       <c r="M58" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>56</v>
       </c>
       <c r="B59" s="2">
         <v>6</v>
       </c>
-      <c r="C59" s="3">
+      <c r="C59">
         <v>13</v>
       </c>
       <c r="D59" s="1">
@@ -3315,7 +3328,7 @@
       <c r="E59" s="2">
         <v>10</v>
       </c>
-      <c r="F59" s="3">
+      <c r="F59">
         <v>10</v>
       </c>
       <c r="G59" s="1">
@@ -3324,7 +3337,7 @@
       <c r="H59" s="2">
         <v>15</v>
       </c>
-      <c r="I59" s="3">
+      <c r="I59">
         <v>14</v>
       </c>
       <c r="J59" s="1">
@@ -3333,21 +3346,21 @@
       <c r="K59" s="2">
         <v>1</v>
       </c>
-      <c r="L59" s="3">
+      <c r="L59">
         <v>1</v>
       </c>
       <c r="M59" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>57</v>
       </c>
       <c r="B60" s="2">
         <v>14</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C60">
         <v>11</v>
       </c>
       <c r="D60" s="1">
@@ -3356,7 +3369,7 @@
       <c r="E60" s="2">
         <v>13</v>
       </c>
-      <c r="F60" s="3">
+      <c r="F60">
         <v>14</v>
       </c>
       <c r="G60" s="1">
@@ -3365,7 +3378,7 @@
       <c r="H60" s="2">
         <v>8</v>
       </c>
-      <c r="I60" s="3">
+      <c r="I60">
         <v>12</v>
       </c>
       <c r="J60" s="1">
@@ -3374,21 +3387,21 @@
       <c r="K60" s="2">
         <v>1</v>
       </c>
-      <c r="L60" s="3">
+      <c r="L60">
         <v>1</v>
       </c>
       <c r="M60" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>58</v>
       </c>
       <c r="B61" s="2">
         <v>7</v>
       </c>
-      <c r="C61" s="3">
+      <c r="C61">
         <v>17</v>
       </c>
       <c r="D61" s="1">
@@ -3397,7 +3410,7 @@
       <c r="E61" s="2">
         <v>8</v>
       </c>
-      <c r="F61" s="3">
+      <c r="F61">
         <v>13</v>
       </c>
       <c r="G61" s="1">
@@ -3406,7 +3419,7 @@
       <c r="H61" s="2">
         <v>13</v>
       </c>
-      <c r="I61" s="3">
+      <c r="I61">
         <v>15</v>
       </c>
       <c r="J61" s="1">
@@ -3415,21 +3428,21 @@
       <c r="K61" s="2">
         <v>1</v>
       </c>
-      <c r="L61" s="3">
+      <c r="L61">
         <v>1</v>
       </c>
       <c r="M61" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>59</v>
       </c>
       <c r="B62" s="2">
         <v>12</v>
       </c>
-      <c r="C62" s="3">
+      <c r="C62">
         <v>17</v>
       </c>
       <c r="D62" s="1">
@@ -3438,7 +3451,7 @@
       <c r="E62" s="2">
         <v>13</v>
       </c>
-      <c r="F62" s="3">
+      <c r="F62">
         <v>14</v>
       </c>
       <c r="G62" s="1">
@@ -3447,7 +3460,7 @@
       <c r="H62" s="2">
         <v>11</v>
       </c>
-      <c r="I62" s="3">
+      <c r="I62">
         <v>10</v>
       </c>
       <c r="J62" s="1">
@@ -3456,21 +3469,21 @@
       <c r="K62" s="2">
         <v>1</v>
       </c>
-      <c r="L62" s="3">
+      <c r="L62">
         <v>2</v>
       </c>
       <c r="M62" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>60</v>
       </c>
       <c r="B63" s="2">
         <v>13</v>
       </c>
-      <c r="C63" s="3">
+      <c r="C63">
         <v>18</v>
       </c>
       <c r="D63" s="1">
@@ -3479,7 +3492,7 @@
       <c r="E63" s="2">
         <v>7</v>
       </c>
-      <c r="F63" s="3">
+      <c r="F63">
         <v>15</v>
       </c>
       <c r="G63" s="1">
@@ -3488,7 +3501,7 @@
       <c r="H63" s="2">
         <v>13</v>
       </c>
-      <c r="I63" s="3">
+      <c r="I63">
         <v>11</v>
       </c>
       <c r="J63" s="1">
@@ -3497,21 +3510,21 @@
       <c r="K63" s="2">
         <v>3</v>
       </c>
-      <c r="L63" s="3">
+      <c r="L63">
         <v>2</v>
       </c>
       <c r="M63" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>61</v>
       </c>
       <c r="B64" s="2">
         <v>12</v>
       </c>
-      <c r="C64" s="3">
+      <c r="C64">
         <v>17</v>
       </c>
       <c r="D64" s="1">
@@ -3520,7 +3533,7 @@
       <c r="E64" s="2">
         <v>11</v>
       </c>
-      <c r="F64" s="3">
+      <c r="F64">
         <v>10</v>
       </c>
       <c r="G64" s="1">
@@ -3529,7 +3542,7 @@
       <c r="H64" s="2">
         <v>14</v>
       </c>
-      <c r="I64" s="3">
+      <c r="I64">
         <v>16</v>
       </c>
       <c r="J64" s="1">
@@ -3538,21 +3551,21 @@
       <c r="K64" s="2">
         <v>3</v>
       </c>
-      <c r="L64" s="3">
+      <c r="L64">
         <v>3</v>
       </c>
       <c r="M64" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>62</v>
       </c>
       <c r="B65" s="2">
         <v>8</v>
       </c>
-      <c r="C65" s="3">
+      <c r="C65">
         <v>20</v>
       </c>
       <c r="D65" s="1">
@@ -3561,7 +3574,7 @@
       <c r="E65" s="2">
         <v>15</v>
       </c>
-      <c r="F65" s="3">
+      <c r="F65">
         <v>11</v>
       </c>
       <c r="G65" s="1">
@@ -3570,7 +3583,7 @@
       <c r="H65" s="2">
         <v>15</v>
       </c>
-      <c r="I65" s="3">
+      <c r="I65">
         <v>14</v>
       </c>
       <c r="J65" s="1">
@@ -3579,21 +3592,21 @@
       <c r="K65" s="2">
         <v>3</v>
       </c>
-      <c r="L65" s="3">
+      <c r="L65">
         <v>1</v>
       </c>
       <c r="M65" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>63</v>
       </c>
       <c r="B66" s="2">
         <v>14</v>
       </c>
-      <c r="C66" s="3">
+      <c r="C66">
         <v>20</v>
       </c>
       <c r="D66" s="1">
@@ -3602,7 +3615,7 @@
       <c r="E66" s="2">
         <v>6</v>
       </c>
-      <c r="F66" s="3">
+      <c r="F66">
         <v>13</v>
       </c>
       <c r="G66" s="1">
@@ -3611,7 +3624,7 @@
       <c r="H66" s="2">
         <v>7</v>
       </c>
-      <c r="I66" s="3">
+      <c r="I66">
         <v>13</v>
       </c>
       <c r="J66" s="1">
@@ -3620,21 +3633,21 @@
       <c r="K66" s="2">
         <v>1</v>
       </c>
-      <c r="L66" s="3">
+      <c r="L66">
         <v>1</v>
       </c>
       <c r="M66" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>64</v>
       </c>
       <c r="B67" s="2">
         <v>15</v>
       </c>
-      <c r="C67" s="3">
+      <c r="C67">
         <v>16</v>
       </c>
       <c r="D67" s="1">
@@ -3643,7 +3656,7 @@
       <c r="E67" s="2">
         <v>15</v>
       </c>
-      <c r="F67" s="3">
+      <c r="F67">
         <v>11</v>
       </c>
       <c r="G67" s="1">
@@ -3652,7 +3665,7 @@
       <c r="H67" s="2">
         <v>8</v>
       </c>
-      <c r="I67" s="3">
+      <c r="I67">
         <v>19</v>
       </c>
       <c r="J67" s="1">
@@ -3661,21 +3674,21 @@
       <c r="K67" s="2">
         <v>3</v>
       </c>
-      <c r="L67" s="3">
+      <c r="L67">
         <v>1</v>
       </c>
       <c r="M67" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>65</v>
       </c>
       <c r="B68" s="2">
         <v>10</v>
       </c>
-      <c r="C68" s="3">
+      <c r="C68">
         <v>14</v>
       </c>
       <c r="D68" s="1">
@@ -3684,7 +3697,7 @@
       <c r="E68" s="2">
         <v>13</v>
       </c>
-      <c r="F68" s="3">
+      <c r="F68">
         <v>14</v>
       </c>
       <c r="G68" s="1">
@@ -3693,7 +3706,7 @@
       <c r="H68" s="2">
         <v>15</v>
       </c>
-      <c r="I68" s="3">
+      <c r="I68">
         <v>17</v>
       </c>
       <c r="J68" s="1">
@@ -3702,21 +3715,21 @@
       <c r="K68" s="2">
         <v>1</v>
       </c>
-      <c r="L68" s="3">
+      <c r="L68">
         <v>1</v>
       </c>
       <c r="M68" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>66</v>
       </c>
       <c r="B69" s="2">
         <v>12</v>
       </c>
-      <c r="C69" s="3">
+      <c r="C69">
         <v>17</v>
       </c>
       <c r="D69" s="1">
@@ -3725,7 +3738,7 @@
       <c r="E69" s="2">
         <v>7</v>
       </c>
-      <c r="F69" s="3">
+      <c r="F69">
         <v>18</v>
       </c>
       <c r="G69" s="1">
@@ -3734,7 +3747,7 @@
       <c r="H69" s="2">
         <v>7</v>
       </c>
-      <c r="I69" s="3">
+      <c r="I69">
         <v>17</v>
       </c>
       <c r="J69" s="1">
@@ -3743,21 +3756,21 @@
       <c r="K69" s="2">
         <v>2</v>
       </c>
-      <c r="L69" s="3">
+      <c r="L69">
         <v>2</v>
       </c>
       <c r="M69" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>67</v>
       </c>
       <c r="B70" s="2">
         <v>13</v>
       </c>
-      <c r="C70" s="3">
+      <c r="C70">
         <v>15</v>
       </c>
       <c r="D70" s="1">
@@ -3766,7 +3779,7 @@
       <c r="E70" s="2">
         <v>9</v>
       </c>
-      <c r="F70" s="3">
+      <c r="F70">
         <v>16</v>
       </c>
       <c r="G70" s="1">
@@ -3775,7 +3788,7 @@
       <c r="H70" s="2">
         <v>8</v>
       </c>
-      <c r="I70" s="3">
+      <c r="I70">
         <v>20</v>
       </c>
       <c r="J70" s="1">
@@ -3784,21 +3797,21 @@
       <c r="K70" s="2">
         <v>1</v>
       </c>
-      <c r="L70" s="3">
+      <c r="L70">
         <v>2</v>
       </c>
       <c r="M70" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>68</v>
       </c>
       <c r="B71" s="2">
         <v>7</v>
       </c>
-      <c r="C71" s="3">
+      <c r="C71">
         <v>15</v>
       </c>
       <c r="D71" s="1">
@@ -3807,7 +3820,7 @@
       <c r="E71" s="2">
         <v>15</v>
       </c>
-      <c r="F71" s="3">
+      <c r="F71">
         <v>13</v>
       </c>
       <c r="G71" s="1">
@@ -3816,7 +3829,7 @@
       <c r="H71" s="2">
         <v>15</v>
       </c>
-      <c r="I71" s="3">
+      <c r="I71">
         <v>16</v>
       </c>
       <c r="J71" s="1">
@@ -3825,21 +3838,21 @@
       <c r="K71" s="2">
         <v>1</v>
       </c>
-      <c r="L71" s="3">
+      <c r="L71">
         <v>2</v>
       </c>
       <c r="M71" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>69</v>
       </c>
       <c r="B72" s="2">
         <v>8</v>
       </c>
-      <c r="C72" s="3">
+      <c r="C72">
         <v>13</v>
       </c>
       <c r="D72" s="1">
@@ -3848,7 +3861,7 @@
       <c r="E72" s="2">
         <v>15</v>
       </c>
-      <c r="F72" s="3">
+      <c r="F72">
         <v>20</v>
       </c>
       <c r="G72" s="1">
@@ -3857,7 +3870,7 @@
       <c r="H72" s="2">
         <v>12</v>
       </c>
-      <c r="I72" s="3">
+      <c r="I72">
         <v>10</v>
       </c>
       <c r="J72" s="1">
@@ -3866,21 +3879,21 @@
       <c r="K72" s="2">
         <v>3</v>
       </c>
-      <c r="L72" s="3">
+      <c r="L72">
         <v>2</v>
       </c>
       <c r="M72" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>70</v>
       </c>
       <c r="B73" s="2">
         <v>12</v>
       </c>
-      <c r="C73" s="3">
+      <c r="C73">
         <v>18</v>
       </c>
       <c r="D73" s="1">
@@ -3889,7 +3902,7 @@
       <c r="E73" s="2">
         <v>9</v>
       </c>
-      <c r="F73" s="3">
+      <c r="F73">
         <v>14</v>
       </c>
       <c r="G73" s="1">
@@ -3898,7 +3911,7 @@
       <c r="H73" s="2">
         <v>11</v>
       </c>
-      <c r="I73" s="3">
+      <c r="I73">
         <v>17</v>
       </c>
       <c r="J73" s="1">
@@ -3907,21 +3920,21 @@
       <c r="K73" s="2">
         <v>3</v>
       </c>
-      <c r="L73" s="3">
+      <c r="L73">
         <v>1</v>
       </c>
       <c r="M73" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>71</v>
       </c>
       <c r="B74" s="2">
         <v>14</v>
       </c>
-      <c r="C74" s="3">
+      <c r="C74">
         <v>12</v>
       </c>
       <c r="D74" s="1">
@@ -3930,7 +3943,7 @@
       <c r="E74" s="2">
         <v>13</v>
       </c>
-      <c r="F74" s="3">
+      <c r="F74">
         <v>12</v>
       </c>
       <c r="G74" s="1">
@@ -3939,7 +3952,7 @@
       <c r="H74" s="2">
         <v>15</v>
       </c>
-      <c r="I74" s="3">
+      <c r="I74">
         <v>18</v>
       </c>
       <c r="J74" s="1">
@@ -3948,21 +3961,21 @@
       <c r="K74" s="2">
         <v>2</v>
       </c>
-      <c r="L74" s="3">
+      <c r="L74">
         <v>2</v>
       </c>
       <c r="M74" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>72</v>
       </c>
       <c r="B75" s="2">
         <v>7</v>
       </c>
-      <c r="C75" s="3">
+      <c r="C75">
         <v>20</v>
       </c>
       <c r="D75" s="1">
@@ -3971,7 +3984,7 @@
       <c r="E75" s="2">
         <v>8</v>
       </c>
-      <c r="F75" s="3">
+      <c r="F75">
         <v>19</v>
       </c>
       <c r="G75" s="1">
@@ -3980,7 +3993,7 @@
       <c r="H75" s="2">
         <v>12</v>
       </c>
-      <c r="I75" s="3">
+      <c r="I75">
         <v>10</v>
       </c>
       <c r="J75" s="1">
@@ -3989,21 +4002,21 @@
       <c r="K75" s="2">
         <v>3</v>
       </c>
-      <c r="L75" s="3">
+      <c r="L75">
         <v>2</v>
       </c>
       <c r="M75" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>73</v>
       </c>
       <c r="B76" s="2">
         <v>15</v>
       </c>
-      <c r="C76" s="3">
+      <c r="C76">
         <v>12</v>
       </c>
       <c r="D76" s="1">
@@ -4012,7 +4025,7 @@
       <c r="E76" s="2">
         <v>15</v>
       </c>
-      <c r="F76" s="3">
+      <c r="F76">
         <v>13</v>
       </c>
       <c r="G76" s="1">
@@ -4021,7 +4034,7 @@
       <c r="H76" s="2">
         <v>12</v>
       </c>
-      <c r="I76" s="3">
+      <c r="I76">
         <v>17</v>
       </c>
       <c r="J76" s="1">
@@ -4030,21 +4043,21 @@
       <c r="K76" s="2">
         <v>1</v>
       </c>
-      <c r="L76" s="3">
+      <c r="L76">
         <v>3</v>
       </c>
       <c r="M76" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>74</v>
       </c>
       <c r="B77" s="2">
         <v>7</v>
       </c>
-      <c r="C77" s="3">
+      <c r="C77">
         <v>16</v>
       </c>
       <c r="D77" s="1">
@@ -4053,7 +4066,7 @@
       <c r="E77" s="2">
         <v>15</v>
       </c>
-      <c r="F77" s="3">
+      <c r="F77">
         <v>10</v>
       </c>
       <c r="G77" s="1">
@@ -4062,7 +4075,7 @@
       <c r="H77" s="2">
         <v>9</v>
       </c>
-      <c r="I77" s="3">
+      <c r="I77">
         <v>10</v>
       </c>
       <c r="J77" s="1">
@@ -4071,21 +4084,21 @@
       <c r="K77" s="2">
         <v>1</v>
       </c>
-      <c r="L77" s="3">
+      <c r="L77">
         <v>3</v>
       </c>
       <c r="M77" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>75</v>
       </c>
       <c r="B78" s="2">
         <v>10</v>
       </c>
-      <c r="C78" s="3">
+      <c r="C78">
         <v>14</v>
       </c>
       <c r="D78" s="1">
@@ -4094,7 +4107,7 @@
       <c r="E78" s="2">
         <v>7</v>
       </c>
-      <c r="F78" s="3">
+      <c r="F78">
         <v>11</v>
       </c>
       <c r="G78" s="1">
@@ -4103,7 +4116,7 @@
       <c r="H78" s="2">
         <v>10</v>
       </c>
-      <c r="I78" s="3">
+      <c r="I78">
         <v>17</v>
       </c>
       <c r="J78" s="1">
@@ -4112,21 +4125,21 @@
       <c r="K78" s="2">
         <v>2</v>
       </c>
-      <c r="L78" s="3">
+      <c r="L78">
         <v>2</v>
       </c>
       <c r="M78" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>76</v>
       </c>
       <c r="B79" s="2">
         <v>15</v>
       </c>
-      <c r="C79" s="3">
+      <c r="C79">
         <v>13</v>
       </c>
       <c r="D79" s="1">
@@ -4135,7 +4148,7 @@
       <c r="E79" s="2">
         <v>14</v>
       </c>
-      <c r="F79" s="3">
+      <c r="F79">
         <v>20</v>
       </c>
       <c r="G79" s="1">
@@ -4144,7 +4157,7 @@
       <c r="H79" s="2">
         <v>11</v>
       </c>
-      <c r="I79" s="3">
+      <c r="I79">
         <v>10</v>
       </c>
       <c r="J79" s="1">
@@ -4153,21 +4166,21 @@
       <c r="K79" s="2">
         <v>3</v>
       </c>
-      <c r="L79" s="3">
+      <c r="L79">
         <v>1</v>
       </c>
       <c r="M79" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>77</v>
       </c>
       <c r="B80" s="2">
         <v>12</v>
       </c>
-      <c r="C80" s="3">
+      <c r="C80">
         <v>14</v>
       </c>
       <c r="D80" s="1">
@@ -4176,7 +4189,7 @@
       <c r="E80" s="2">
         <v>12</v>
       </c>
-      <c r="F80" s="3">
+      <c r="F80">
         <v>16</v>
       </c>
       <c r="G80" s="1">
@@ -4185,7 +4198,7 @@
       <c r="H80" s="2">
         <v>14</v>
       </c>
-      <c r="I80" s="3">
+      <c r="I80">
         <v>19</v>
       </c>
       <c r="J80" s="1">
@@ -4194,21 +4207,21 @@
       <c r="K80" s="2">
         <v>3</v>
       </c>
-      <c r="L80" s="3">
+      <c r="L80">
         <v>2</v>
       </c>
       <c r="M80" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>78</v>
       </c>
       <c r="B81" s="2">
         <v>14</v>
       </c>
-      <c r="C81" s="3">
+      <c r="C81">
         <v>13</v>
       </c>
       <c r="D81" s="1">
@@ -4217,7 +4230,7 @@
       <c r="E81" s="2">
         <v>7</v>
       </c>
-      <c r="F81" s="3">
+      <c r="F81">
         <v>16</v>
       </c>
       <c r="G81" s="1">
@@ -4226,7 +4239,7 @@
       <c r="H81" s="2">
         <v>12</v>
       </c>
-      <c r="I81" s="3">
+      <c r="I81">
         <v>13</v>
       </c>
       <c r="J81" s="1">
@@ -4235,21 +4248,21 @@
       <c r="K81" s="2">
         <v>3</v>
       </c>
-      <c r="L81" s="3">
+      <c r="L81">
         <v>2</v>
       </c>
       <c r="M81" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>79</v>
       </c>
       <c r="B82" s="2">
         <v>6</v>
       </c>
-      <c r="C82" s="3">
+      <c r="C82">
         <v>18</v>
       </c>
       <c r="D82" s="1">
@@ -4258,7 +4271,7 @@
       <c r="E82" s="2">
         <v>6</v>
       </c>
-      <c r="F82" s="3">
+      <c r="F82">
         <v>18</v>
       </c>
       <c r="G82" s="1">
@@ -4267,7 +4280,7 @@
       <c r="H82" s="2">
         <v>12</v>
       </c>
-      <c r="I82" s="3">
+      <c r="I82">
         <v>17</v>
       </c>
       <c r="J82" s="1">
@@ -4276,21 +4289,21 @@
       <c r="K82" s="2">
         <v>3</v>
       </c>
-      <c r="L82" s="3">
+      <c r="L82">
         <v>2</v>
       </c>
       <c r="M82" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>80</v>
       </c>
       <c r="B83" s="2">
         <v>7</v>
       </c>
-      <c r="C83" s="3">
+      <c r="C83">
         <v>13</v>
       </c>
       <c r="D83" s="1">
@@ -4299,7 +4312,7 @@
       <c r="E83" s="2">
         <v>15</v>
       </c>
-      <c r="F83" s="3">
+      <c r="F83">
         <v>16</v>
       </c>
       <c r="G83" s="1">
@@ -4308,7 +4321,7 @@
       <c r="H83" s="2">
         <v>9</v>
       </c>
-      <c r="I83" s="3">
+      <c r="I83">
         <v>15</v>
       </c>
       <c r="J83" s="1">
@@ -4317,21 +4330,21 @@
       <c r="K83" s="2">
         <v>2</v>
       </c>
-      <c r="L83" s="3">
+      <c r="L83">
         <v>2</v>
       </c>
       <c r="M83" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>81</v>
       </c>
       <c r="B84" s="2">
         <v>11</v>
       </c>
-      <c r="C84" s="3">
+      <c r="C84">
         <v>10</v>
       </c>
       <c r="D84" s="1">
@@ -4340,7 +4353,7 @@
       <c r="E84" s="2">
         <v>12</v>
       </c>
-      <c r="F84" s="3">
+      <c r="F84">
         <v>11</v>
       </c>
       <c r="G84" s="1">
@@ -4349,7 +4362,7 @@
       <c r="H84" s="2">
         <v>6</v>
       </c>
-      <c r="I84" s="3">
+      <c r="I84">
         <v>11</v>
       </c>
       <c r="J84" s="1">
@@ -4358,21 +4371,21 @@
       <c r="K84" s="2">
         <v>3</v>
       </c>
-      <c r="L84" s="3">
+      <c r="L84">
         <v>2</v>
       </c>
       <c r="M84" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>82</v>
       </c>
       <c r="B85" s="2">
         <v>12</v>
       </c>
-      <c r="C85" s="3">
+      <c r="C85">
         <v>12</v>
       </c>
       <c r="D85" s="1">
@@ -4381,7 +4394,7 @@
       <c r="E85" s="2">
         <v>6</v>
       </c>
-      <c r="F85" s="3">
+      <c r="F85">
         <v>14</v>
       </c>
       <c r="G85" s="1">
@@ -4390,7 +4403,7 @@
       <c r="H85" s="2">
         <v>14</v>
       </c>
-      <c r="I85" s="3">
+      <c r="I85">
         <v>12</v>
       </c>
       <c r="J85" s="1">
@@ -4399,21 +4412,21 @@
       <c r="K85" s="2">
         <v>3</v>
       </c>
-      <c r="L85" s="3">
+      <c r="L85">
         <v>3</v>
       </c>
       <c r="M85" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>83</v>
       </c>
       <c r="B86" s="2">
         <v>7</v>
       </c>
-      <c r="C86" s="3">
+      <c r="C86">
         <v>14</v>
       </c>
       <c r="D86" s="1">
@@ -4422,7 +4435,7 @@
       <c r="E86" s="2">
         <v>13</v>
       </c>
-      <c r="F86" s="3">
+      <c r="F86">
         <v>11</v>
       </c>
       <c r="G86" s="1">
@@ -4431,7 +4444,7 @@
       <c r="H86" s="2">
         <v>12</v>
       </c>
-      <c r="I86" s="3">
+      <c r="I86">
         <v>20</v>
       </c>
       <c r="J86" s="1">
@@ -4440,21 +4453,21 @@
       <c r="K86" s="2">
         <v>3</v>
       </c>
-      <c r="L86" s="3">
+      <c r="L86">
         <v>2</v>
       </c>
       <c r="M86" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>84</v>
       </c>
       <c r="B87" s="2">
         <v>9</v>
       </c>
-      <c r="C87" s="3">
+      <c r="C87">
         <v>18</v>
       </c>
       <c r="D87" s="1">
@@ -4463,7 +4476,7 @@
       <c r="E87" s="2">
         <v>6</v>
       </c>
-      <c r="F87" s="3">
+      <c r="F87">
         <v>11</v>
       </c>
       <c r="G87" s="1">
@@ -4472,7 +4485,7 @@
       <c r="H87" s="2">
         <v>15</v>
       </c>
-      <c r="I87" s="3">
+      <c r="I87">
         <v>16</v>
       </c>
       <c r="J87" s="1">
@@ -4481,21 +4494,21 @@
       <c r="K87" s="2">
         <v>2</v>
       </c>
-      <c r="L87" s="3">
+      <c r="L87">
         <v>2</v>
       </c>
       <c r="M87" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>85</v>
       </c>
       <c r="B88" s="2">
         <v>15</v>
       </c>
-      <c r="C88" s="3">
+      <c r="C88">
         <v>18</v>
       </c>
       <c r="D88" s="1">
@@ -4504,7 +4517,7 @@
       <c r="E88" s="2">
         <v>11</v>
       </c>
-      <c r="F88" s="3">
+      <c r="F88">
         <v>10</v>
       </c>
       <c r="G88" s="1">
@@ -4513,7 +4526,7 @@
       <c r="H88" s="2">
         <v>12</v>
       </c>
-      <c r="I88" s="3">
+      <c r="I88">
         <v>11</v>
       </c>
       <c r="J88" s="1">
@@ -4522,21 +4535,21 @@
       <c r="K88" s="2">
         <v>1</v>
       </c>
-      <c r="L88" s="3">
+      <c r="L88">
         <v>1</v>
       </c>
       <c r="M88" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>86</v>
       </c>
       <c r="B89" s="2">
         <v>8</v>
       </c>
-      <c r="C89" s="3">
+      <c r="C89">
         <v>20</v>
       </c>
       <c r="D89" s="1">
@@ -4545,7 +4558,7 @@
       <c r="E89" s="2">
         <v>11</v>
       </c>
-      <c r="F89" s="3">
+      <c r="F89">
         <v>18</v>
       </c>
       <c r="G89" s="1">
@@ -4554,7 +4567,7 @@
       <c r="H89" s="2">
         <v>8</v>
       </c>
-      <c r="I89" s="3">
+      <c r="I89">
         <v>15</v>
       </c>
       <c r="J89" s="1">
@@ -4563,21 +4576,21 @@
       <c r="K89" s="2">
         <v>2</v>
       </c>
-      <c r="L89" s="3">
+      <c r="L89">
         <v>2</v>
       </c>
       <c r="M89" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>87</v>
       </c>
       <c r="B90" s="2">
         <v>7</v>
       </c>
-      <c r="C90" s="3">
+      <c r="C90">
         <v>18</v>
       </c>
       <c r="D90" s="1">
@@ -4586,7 +4599,7 @@
       <c r="E90" s="2">
         <v>14</v>
       </c>
-      <c r="F90" s="3">
+      <c r="F90">
         <v>13</v>
       </c>
       <c r="G90" s="1">
@@ -4595,7 +4608,7 @@
       <c r="H90" s="2">
         <v>7</v>
       </c>
-      <c r="I90" s="3">
+      <c r="I90">
         <v>11</v>
       </c>
       <c r="J90" s="1">
@@ -4604,21 +4617,21 @@
       <c r="K90" s="2">
         <v>3</v>
       </c>
-      <c r="L90" s="3">
+      <c r="L90">
         <v>2</v>
       </c>
       <c r="M90" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>88</v>
       </c>
       <c r="B91" s="2">
         <v>6</v>
       </c>
-      <c r="C91" s="3">
+      <c r="C91">
         <v>10</v>
       </c>
       <c r="D91" s="1">
@@ -4627,7 +4640,7 @@
       <c r="E91" s="2">
         <v>6</v>
       </c>
-      <c r="F91" s="3">
+      <c r="F91">
         <v>17</v>
       </c>
       <c r="G91" s="1">
@@ -4636,7 +4649,7 @@
       <c r="H91" s="2">
         <v>15</v>
       </c>
-      <c r="I91" s="3">
+      <c r="I91">
         <v>19</v>
       </c>
       <c r="J91" s="1">
@@ -4645,21 +4658,21 @@
       <c r="K91" s="2">
         <v>1</v>
       </c>
-      <c r="L91" s="3">
+      <c r="L91">
         <v>3</v>
       </c>
       <c r="M91" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>89</v>
       </c>
       <c r="B92" s="2">
         <v>10</v>
       </c>
-      <c r="C92" s="3">
+      <c r="C92">
         <v>19</v>
       </c>
       <c r="D92" s="1">
@@ -4668,7 +4681,7 @@
       <c r="E92" s="2">
         <v>15</v>
       </c>
-      <c r="F92" s="3">
+      <c r="F92">
         <v>12</v>
       </c>
       <c r="G92" s="1">
@@ -4677,7 +4690,7 @@
       <c r="H92" s="2">
         <v>13</v>
       </c>
-      <c r="I92" s="3">
+      <c r="I92">
         <v>20</v>
       </c>
       <c r="J92" s="1">
@@ -4686,21 +4699,21 @@
       <c r="K92" s="2">
         <v>2</v>
       </c>
-      <c r="L92" s="3">
+      <c r="L92">
         <v>2</v>
       </c>
       <c r="M92" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>90</v>
       </c>
       <c r="B93" s="2">
         <v>15</v>
       </c>
-      <c r="C93" s="3">
+      <c r="C93">
         <v>19</v>
       </c>
       <c r="D93" s="1">
@@ -4709,7 +4722,7 @@
       <c r="E93" s="2">
         <v>9</v>
       </c>
-      <c r="F93" s="3">
+      <c r="F93">
         <v>20</v>
       </c>
       <c r="G93" s="1">
@@ -4718,7 +4731,7 @@
       <c r="H93" s="2">
         <v>10</v>
       </c>
-      <c r="I93" s="3">
+      <c r="I93">
         <v>20</v>
       </c>
       <c r="J93" s="1">
@@ -4727,21 +4740,21 @@
       <c r="K93" s="2">
         <v>1</v>
       </c>
-      <c r="L93" s="3">
+      <c r="L93">
         <v>1</v>
       </c>
       <c r="M93" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>91</v>
       </c>
       <c r="B94" s="2">
         <v>10</v>
       </c>
-      <c r="C94" s="3">
+      <c r="C94">
         <v>11</v>
       </c>
       <c r="D94" s="1">
@@ -4750,7 +4763,7 @@
       <c r="E94" s="2">
         <v>14</v>
       </c>
-      <c r="F94" s="3">
+      <c r="F94">
         <v>20</v>
       </c>
       <c r="G94" s="1">
@@ -4759,7 +4772,7 @@
       <c r="H94" s="2">
         <v>9</v>
       </c>
-      <c r="I94" s="3">
+      <c r="I94">
         <v>19</v>
       </c>
       <c r="J94" s="1">
@@ -4768,21 +4781,21 @@
       <c r="K94" s="2">
         <v>2</v>
       </c>
-      <c r="L94" s="3">
+      <c r="L94">
         <v>1</v>
       </c>
       <c r="M94" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>92</v>
       </c>
       <c r="B95" s="2">
         <v>15</v>
       </c>
-      <c r="C95" s="3">
+      <c r="C95">
         <v>14</v>
       </c>
       <c r="D95" s="1">
@@ -4791,7 +4804,7 @@
       <c r="E95" s="2">
         <v>12</v>
       </c>
-      <c r="F95" s="3">
+      <c r="F95">
         <v>20</v>
       </c>
       <c r="G95" s="1">
@@ -4800,7 +4813,7 @@
       <c r="H95" s="2">
         <v>15</v>
       </c>
-      <c r="I95" s="3">
+      <c r="I95">
         <v>20</v>
       </c>
       <c r="J95" s="1">
@@ -4809,21 +4822,21 @@
       <c r="K95" s="2">
         <v>1</v>
       </c>
-      <c r="L95" s="3">
+      <c r="L95">
         <v>3</v>
       </c>
       <c r="M95" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>93</v>
       </c>
       <c r="B96" s="2">
         <v>6</v>
       </c>
-      <c r="C96" s="3">
+      <c r="C96">
         <v>15</v>
       </c>
       <c r="D96" s="1">
@@ -4832,7 +4845,7 @@
       <c r="E96" s="2">
         <v>10</v>
       </c>
-      <c r="F96" s="3">
+      <c r="F96">
         <v>19</v>
       </c>
       <c r="G96" s="1">
@@ -4841,7 +4854,7 @@
       <c r="H96" s="2">
         <v>7</v>
       </c>
-      <c r="I96" s="3">
+      <c r="I96">
         <v>12</v>
       </c>
       <c r="J96" s="1">
@@ -4850,21 +4863,21 @@
       <c r="K96" s="2">
         <v>2</v>
       </c>
-      <c r="L96" s="3">
+      <c r="L96">
         <v>2</v>
       </c>
       <c r="M96" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>94</v>
       </c>
       <c r="B97" s="2">
         <v>7</v>
       </c>
-      <c r="C97" s="3">
+      <c r="C97">
         <v>14</v>
       </c>
       <c r="D97" s="1">
@@ -4873,7 +4886,7 @@
       <c r="E97" s="2">
         <v>7</v>
       </c>
-      <c r="F97" s="3">
+      <c r="F97">
         <v>10</v>
       </c>
       <c r="G97" s="1">
@@ -4882,7 +4895,7 @@
       <c r="H97" s="2">
         <v>15</v>
       </c>
-      <c r="I97" s="3">
+      <c r="I97">
         <v>19</v>
       </c>
       <c r="J97" s="1">
@@ -4891,21 +4904,21 @@
       <c r="K97" s="2">
         <v>2</v>
       </c>
-      <c r="L97" s="3">
+      <c r="L97">
         <v>1</v>
       </c>
       <c r="M97" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>95</v>
       </c>
       <c r="B98" s="2">
         <v>14</v>
       </c>
-      <c r="C98" s="3">
+      <c r="C98">
         <v>10</v>
       </c>
       <c r="D98" s="1">
@@ -4914,7 +4927,7 @@
       <c r="E98" s="2">
         <v>8</v>
       </c>
-      <c r="F98" s="3">
+      <c r="F98">
         <v>20</v>
       </c>
       <c r="G98" s="1">
@@ -4923,7 +4936,7 @@
       <c r="H98" s="2">
         <v>9</v>
       </c>
-      <c r="I98" s="3">
+      <c r="I98">
         <v>19</v>
       </c>
       <c r="J98" s="1">
@@ -4932,21 +4945,21 @@
       <c r="K98" s="2">
         <v>1</v>
       </c>
-      <c r="L98" s="3">
+      <c r="L98">
         <v>2</v>
       </c>
       <c r="M98" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>96</v>
       </c>
       <c r="B99" s="2">
         <v>11</v>
       </c>
-      <c r="C99" s="3">
+      <c r="C99">
         <v>19</v>
       </c>
       <c r="D99" s="1">
@@ -4955,7 +4968,7 @@
       <c r="E99" s="2">
         <v>14</v>
       </c>
-      <c r="F99" s="3">
+      <c r="F99">
         <v>14</v>
       </c>
       <c r="G99" s="1">
@@ -4964,7 +4977,7 @@
       <c r="H99" s="2">
         <v>15</v>
       </c>
-      <c r="I99" s="3">
+      <c r="I99">
         <v>12</v>
       </c>
       <c r="J99" s="1">
@@ -4973,21 +4986,21 @@
       <c r="K99" s="2">
         <v>2</v>
       </c>
-      <c r="L99" s="3">
+      <c r="L99">
         <v>2</v>
       </c>
       <c r="M99" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>97</v>
       </c>
       <c r="B100" s="2">
         <v>6</v>
       </c>
-      <c r="C100" s="3">
+      <c r="C100">
         <v>12</v>
       </c>
       <c r="D100" s="1">
@@ -4996,7 +5009,7 @@
       <c r="E100" s="2">
         <v>9</v>
       </c>
-      <c r="F100" s="3">
+      <c r="F100">
         <v>11</v>
       </c>
       <c r="G100" s="1">
@@ -5005,7 +5018,7 @@
       <c r="H100" s="2">
         <v>10</v>
       </c>
-      <c r="I100" s="3">
+      <c r="I100">
         <v>15</v>
       </c>
       <c r="J100" s="1">
@@ -5014,21 +5027,21 @@
       <c r="K100" s="2">
         <v>1</v>
       </c>
-      <c r="L100" s="3">
+      <c r="L100">
         <v>1</v>
       </c>
       <c r="M100" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>98</v>
       </c>
       <c r="B101" s="2">
         <v>15</v>
       </c>
-      <c r="C101" s="3">
+      <c r="C101">
         <v>17</v>
       </c>
       <c r="D101" s="1">
@@ -5037,7 +5050,7 @@
       <c r="E101" s="2">
         <v>6</v>
       </c>
-      <c r="F101" s="3">
+      <c r="F101">
         <v>19</v>
       </c>
       <c r="G101" s="1">
@@ -5046,7 +5059,7 @@
       <c r="H101" s="2">
         <v>10</v>
       </c>
-      <c r="I101" s="3">
+      <c r="I101">
         <v>14</v>
       </c>
       <c r="J101" s="1">
@@ -5055,21 +5068,21 @@
       <c r="K101" s="2">
         <v>1</v>
       </c>
-      <c r="L101" s="3">
+      <c r="L101">
         <v>1</v>
       </c>
       <c r="M101" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>99</v>
       </c>
       <c r="B102" s="2">
         <v>8</v>
       </c>
-      <c r="C102" s="3">
+      <c r="C102">
         <v>10</v>
       </c>
       <c r="D102" s="1">
@@ -5078,7 +5091,7 @@
       <c r="E102" s="2">
         <v>7</v>
       </c>
-      <c r="F102" s="3">
+      <c r="F102">
         <v>19</v>
       </c>
       <c r="G102" s="1">
@@ -5087,7 +5100,7 @@
       <c r="H102" s="2">
         <v>13</v>
       </c>
-      <c r="I102" s="3">
+      <c r="I102">
         <v>14</v>
       </c>
       <c r="J102" s="1">
@@ -5096,7 +5109,7 @@
       <c r="K102" s="2">
         <v>2</v>
       </c>
-      <c r="L102" s="3">
+      <c r="L102">
         <v>3</v>
       </c>
       <c r="M102" s="1">

</xml_diff>